<commit_message>
Added "no floor" nodes
-Created new "no floor" scriptable objects with corresponding prefabs. -Adjusted constraint dictionary to accommodate for new faces
</commit_message>
<xml_diff>
--- a/ProceduralGenerationPrototype/Assets/NodeFaceInfo.xlsx
+++ b/ProceduralGenerationPrototype/Assets/NodeFaceInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive\Documents\GitHub\To-Jonathan-AdvTop24\ProceduralGenerationPrototype\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45F53DED-3CFE-4925-B9F3-62A60668817E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6A00FC-05B7-4AFB-B8D4-5414F4F88476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B954FBA1-4E8E-4196-B0B4-174D3795C96B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>p1</t>
   </si>
@@ -116,12 +116,6 @@
     <t>p26</t>
   </si>
   <si>
-    <t>p27</t>
-  </si>
-  <si>
-    <t>p28</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -174,6 +168,48 @@
   </si>
   <si>
     <t>NegZSymmetric</t>
+  </si>
+  <si>
+    <t>Original Name</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>FL Corner</t>
+  </si>
+  <si>
+    <t>FR Corner</t>
+  </si>
+  <si>
+    <t>LB Corner</t>
+  </si>
+  <si>
+    <t>RB Corner</t>
+  </si>
+  <si>
+    <t>F Wall</t>
+  </si>
+  <si>
+    <t>L Wall</t>
+  </si>
+  <si>
+    <t>R Wall</t>
+  </si>
+  <si>
+    <t>B Wall</t>
+  </si>
+  <si>
+    <t>PosY</t>
+  </si>
+  <si>
+    <t>PosYFlipped</t>
+  </si>
+  <si>
+    <t>PosYSymmetric</t>
   </si>
 </sst>
 </file>
@@ -551,303 +587,704 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7268651E-B372-452A-9602-31D2336BA396}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="10" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>37</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>3</v>
+      </c>
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>-1</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>-1</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>-1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>-1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>-1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>-1</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>-1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>-1</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29">
+      <c r="D27">
         <v>3</v>
       </c>
     </row>

</xml_diff>